<commit_message>
Updated BOMs, cleaned READMEs
</commit_message>
<xml_diff>
--- a/hydraulic_pump/pump_BOM.xlsx
+++ b/hydraulic_pump/pump_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josquintille/Documents/ETHZ/Ultrasound/us_doppler_phantom/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergey\Downloads\dopflow\hydraulic_pump\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB20223-E4B9-FA4F-8687-1892E96F29E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E65000-3227-4330-8022-71B7B695715A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="1420" windowWidth="24640" windowHeight="13500" xr2:uid="{F885F194-4B64-5646-87D2-FC193D84BB8A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F885F194-4B64-5646-87D2-FC193D84BB8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Mechanical" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
   <si>
     <t>Description</t>
   </si>
@@ -85,9 +85,6 @@
     <t>SF2424-10B41</t>
   </si>
   <si>
-    <t>Mouser</t>
-  </si>
-  <si>
     <t xml:space="preserve"> SANMOTION</t>
   </si>
   <si>
@@ -112,33 +109,6 @@
     <t xml:space="preserve">Plastic Syringe, inner diameter is 40 mm, plunge length is 15.5 cm  </t>
   </si>
   <si>
-    <t xml:space="preserve">Mechanical and electrical parts for the velocity controller </t>
-  </si>
-  <si>
-    <t>STMicroelectronics</t>
-  </si>
-  <si>
-    <t>STM32F3DISCOVERY</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ch/ProductDetail/STMicroelectronics/STM32F3DISCOVERY?qs=6ddF3R%2F6EV%2Fl7MfIrXy3BQ%3D%3D</t>
-  </si>
-  <si>
-    <t>MCU board STM32F3DISCOVERY (based on STM32F303VCT6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ARCELI </t>
-  </si>
-  <si>
-    <t>B07MXXL2KW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor driver ARCELI A4988 with Heatsink, 8 to 35V, up to 2 A/phase with cooling and 1 A </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.de/-/en/Compatible-StepStick-Heatsink-Printer-Controller/dp/B07MXXL2KW/ref=sr_1_5?crid=XGSD8ILPXS2X&amp;keywords=A4988&amp;qid=1679330901&amp;sprefix=a4988+%2Caps%2C161&amp;sr=8-5 </t>
-  </si>
-  <si>
     <t>6 mm steel rod to form wall-less phantom</t>
   </si>
   <si>
@@ -299,6 +269,48 @@
   </si>
   <si>
     <t>10min</t>
+  </si>
+  <si>
+    <t>Mechanical and electrical parts for the Hydraulic Pump</t>
+  </si>
+  <si>
+    <t>Flexible Motor Shaft Coupling 6mm to 8mm</t>
+  </si>
+  <si>
+    <t>https://de.aliexpress.com/item/1005006513457969.html?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D19l25 </t>
+  </si>
+  <si>
+    <t>WHOOPEE</t>
+  </si>
+  <si>
+    <t>D19l25 6x8</t>
+  </si>
+  <si>
+    <t>Dowel pins (ISO 2338 ∅4 h6)</t>
+  </si>
+  <si>
+    <t>https://de.aliexpress.com/item/1005007581698118.html</t>
+  </si>
+  <si>
+    <t>GooBetter</t>
+  </si>
+  <si>
+    <t>Diameter 4 mm</t>
+  </si>
+  <si>
+    <t>1 package (7 pins minimum)</t>
+  </si>
+  <si>
+    <t>Screws and washers</t>
+  </si>
+  <si>
+    <t>Steel Hex spacer (M4x12)</t>
+  </si>
+  <si>
+    <t>M3 x 12 &gt; 4 pieces, M4 x 15 &gt; 10 pieces, M3 x 12 &gt; 4 pieces, M5 x 15 &gt; 4 pieces, M6 x 15 &gt; 4 pieces</t>
   </si>
 </sst>
 </file>
@@ -310,7 +322,7 @@
     <numFmt numFmtId="165" formatCode="0\ &quot;m&quot;"/>
     <numFmt numFmtId="166" formatCode="#,##0.00_-\ [$€-1]"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -346,6 +358,16 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -423,10 +445,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -435,25 +457,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="49">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -543,19 +546,38 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -644,19 +666,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{685936D4-299B-2243-A4B1-E6DF62C8CA49}" name="Table1" displayName="Table1" ref="A4:H11" totalsRowCount="1" headerRowDxfId="48" dataDxfId="47">
-  <autoFilter ref="A4:H10" xr:uid="{685936D4-299B-2243-A4B1-E6DF62C8CA49}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{685936D4-299B-2243-A4B1-E6DF62C8CA49}" name="Table1" displayName="Table1" ref="A4:H12" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+  <autoFilter ref="A4:H12" xr:uid="{685936D4-299B-2243-A4B1-E6DF62C8CA49}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C4E14E2B-67AE-9F4F-AEA8-E21C6455E52C}" name="Description" totalsRowLabel="Total" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{C4E14E2B-67AE-9F4F-AEA8-E21C6455E52C}" name="Description" dataDxfId="46" totalsRowDxfId="45"/>
     <tableColumn id="3" xr3:uid="{6907F003-1832-E045-8402-12955C47BAC2}" name="Manufacture" dataDxfId="44" totalsRowDxfId="43"/>
     <tableColumn id="4" xr3:uid="{D17ACCFB-87BB-6048-8F36-11095F20E472}" name="Manufacture Part Number" dataDxfId="42" totalsRowDxfId="41"/>
     <tableColumn id="5" xr3:uid="{D89FB3D7-685C-BA42-BB7D-AE7DC75BF719}" name="Supplier" dataDxfId="40" totalsRowDxfId="39"/>
     <tableColumn id="6" xr3:uid="{8C0DC479-EF54-A841-AEB6-A4545D02941E}" name="Link" dataDxfId="38" totalsRowDxfId="37"/>
     <tableColumn id="7" xr3:uid="{94D5778C-7ABA-3F41-86EB-DC8F035F00F9}" name="Supplier Part Number" dataDxfId="36" totalsRowDxfId="35"/>
     <tableColumn id="8" xr3:uid="{694B9F57-CA19-5445-8BFE-DF960DB2EACE}" name="Supplier Unit Price" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{2D148A4A-93C8-484E-976A-7D8A9CDD80FA}" name="Quantity " totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="31">
-      <totalsRowFormula>SUMPRODUCT(Table1[Supplier Unit Price],Table1[[Quantity ]])</totalsRowFormula>
-    </tableColumn>
+    <tableColumn id="9" xr3:uid="{2D148A4A-93C8-484E-976A-7D8A9CDD80FA}" name="Quantity " dataDxfId="32" totalsRowDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -666,12 +686,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{612431D7-C70C-F645-8CCA-C68521E44550}" name="Table5" displayName="Table5" ref="A3:F12" totalsRowCount="1" headerRowDxfId="30" dataDxfId="29" totalsRowDxfId="28">
   <autoFilter ref="A3:F11" xr:uid="{612431D7-C70C-F645-8CCA-C68521E44550}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{35950D2E-5B90-1E40-8F57-215839D65ED5}" name="Part name" totalsRowLabel="Total" dataDxfId="27" totalsRowDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{409FF984-7B25-BE44-95D1-DA4AD5E531FD}" name="Material" dataDxfId="26" totalsRowDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{194CFE1F-CC2A-274C-9F32-08685EAE6768}" name="Manufacturing methode" dataDxfId="25" totalsRowDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{AF2BDA8D-83B1-7E41-9A0E-C8FAFDC4B856}" name="Manufacturing time" dataDxfId="24" totalsRowDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{5753E5E8-299D-4643-8486-0F9A2CB40F50}" name="number of unit" dataDxfId="23" totalsRowDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{C9F7E48A-FFDF-F348-A2AC-9B4086846031}" name="estimated raw material cost per unit" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="0">
+    <tableColumn id="1" xr3:uid="{35950D2E-5B90-1E40-8F57-215839D65ED5}" name="Part name" totalsRowLabel="Total" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{409FF984-7B25-BE44-95D1-DA4AD5E531FD}" name="Material" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{194CFE1F-CC2A-274C-9F32-08685EAE6768}" name="Manufacturing methode" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{AF2BDA8D-83B1-7E41-9A0E-C8FAFDC4B856}" name="Manufacturing time" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{5753E5E8-299D-4643-8486-0F9A2CB40F50}" name="number of unit" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{C9F7E48A-FFDF-F348-A2AC-9B4086846031}" name="estimated raw material cost per unit" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="16">
       <totalsRowFormula>SUMPRODUCT(Table5[number of unit],Table5[estimated raw material cost per unit])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -680,15 +700,15 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3E382FA9-8A9D-E248-B9E5-3B906B871B12}" name="Table2" displayName="Table2" ref="A4:F11" totalsRowCount="1" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3E382FA9-8A9D-E248-B9E5-3B906B871B12}" name="Table2" displayName="Table2" ref="A4:F11" totalsRowCount="1" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
   <autoFilter ref="A4:F10" xr:uid="{3E382FA9-8A9D-E248-B9E5-3B906B871B12}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E1F28E0D-483E-3044-AC97-19520CA6B64C}" name="Description" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{F3018414-A297-924C-83D9-32872CC33195}" name="Supplier" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{DF64FB3A-4A56-EA46-9E09-5C29895541D9}" name="Link" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{CB539ED9-D1F9-594E-8846-CFC9030D2516}" name="Supplier Part Number" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{5F496FFD-E1D4-E94F-AB0A-C26E7481EF91}" name="Supplier Unit Price" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{08311835-F48E-6B4B-944C-71F252ECBF5D}" name="Quantity " totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
+    <tableColumn id="1" xr3:uid="{E1F28E0D-483E-3044-AC97-19520CA6B64C}" name="Description" totalsRowLabel="Total" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{F3018414-A297-924C-83D9-32872CC33195}" name="Supplier" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{DF64FB3A-4A56-EA46-9E09-5C29895541D9}" name="Link" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{CB539ED9-D1F9-594E-8846-CFC9030D2516}" name="Supplier Part Number" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{5F496FFD-E1D4-E94F-AB0A-C26E7481EF91}" name="Supplier Unit Price" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{08311835-F48E-6B4B-944C-71F252ECBF5D}" name="Quantity " totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
       <totalsRowFormula>SUMPRODUCT(Table2[Supplier Unit Price],Table2[[Quantity ]])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -993,15 +1013,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DC4E19-B466-E144-851E-98FDFB0FA6B6}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="81" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="25.4140625" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" customWidth="1"/>
@@ -1010,21 +1030,21 @@
     <col min="7" max="8" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1050,7 +1070,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1076,21 +1096,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="62" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>14</v>
@@ -1102,136 +1122,139 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="134" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="134" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="G7" s="7">
-        <v>10.99</v>
+        <v>1.4</v>
       </c>
       <c r="H7" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="77" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="134" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>27</v>
+        <v>11</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>84</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="G8" s="7">
-        <v>15.24</v>
-      </c>
-      <c r="H8" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="77" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1.28</v>
+      </c>
+      <c r="H9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="77" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="7">
+        <v>10.99</v>
+      </c>
+      <c r="H10" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="136" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="7">
-        <v>8</v>
-      </c>
-      <c r="H9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="7">
-        <v>1.28</v>
-      </c>
-      <c r="H10" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="77" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="7">
-        <f>SUMPRODUCT(Table1[Supplier Unit Price],Table1[[Quantity ]])</f>
-        <v>111.57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="3"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H12" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1241,7 +1264,7 @@
       <c r="G13" s="7"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1251,7 +1274,7 @@
       <c r="G14" s="7"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1261,7 +1284,7 @@
       <c r="G15" s="7"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1271,7 +1294,7 @@
       <c r="G16" s="7"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1281,7 +1304,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1291,7 +1314,7 @@
       <c r="G18" s="7"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1301,7 +1324,7 @@
       <c r="G19" s="7"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1311,7 +1334,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1321,7 +1344,7 @@
       <c r="G21" s="7"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1331,7 +1354,7 @@
       <c r="G22" s="7"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1341,7 +1364,7 @@
       <c r="G23" s="7"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1351,7 +1374,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1361,7 +1384,7 @@
       <c r="G25" s="7"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1371,7 +1394,7 @@
       <c r="G26" s="7"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1381,7 +1404,7 @@
       <c r="G27" s="7"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1391,7 +1414,7 @@
       <c r="G28" s="7"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1401,7 +1424,7 @@
       <c r="G29" s="7"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1411,7 +1434,7 @@
       <c r="G30" s="7"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1421,7 +1444,7 @@
       <c r="G31" s="7"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1431,7 +1454,7 @@
       <c r="G32" s="7"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1441,7 +1464,7 @@
       <c r="G33" s="7"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1451,7 +1474,7 @@
       <c r="G34" s="7"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1461,7 +1484,7 @@
       <c r="G35" s="7"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1471,7 +1494,7 @@
       <c r="G36" s="7"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1481,7 +1504,7 @@
       <c r="G37" s="7"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1491,7 +1514,7 @@
       <c r="G38" s="7"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1501,7 +1524,7 @@
       <c r="G39" s="7"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1511,7 +1534,7 @@
       <c r="G40" s="7"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1521,7 +1544,7 @@
       <c r="G41" s="7"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1531,7 +1554,7 @@
       <c r="G42" s="7"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1541,7 +1564,7 @@
       <c r="G43" s="7"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1551,7 +1574,7 @@
       <c r="G44" s="7"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1561,6 +1584,16 @@
       <c r="G45" s="7"/>
       <c r="H45" s="3"/>
     </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D2"/>
@@ -1569,12 +1602,12 @@
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{915186C5-0A37-2440-9107-F50340402746}"/>
     <hyperlink ref="E6" r:id="rId2" xr:uid="{FC5FE47C-F72B-804C-8C84-E8E9B84E7D32}"/>
-    <hyperlink ref="E7" r:id="rId3" xr:uid="{F5E38187-B720-694E-8A41-E4D7CEA82071}"/>
-    <hyperlink ref="E8" r:id="rId4" xr:uid="{16F1E677-114F-2E47-95CA-BAB804DCFF9D}"/>
-    <hyperlink ref="E9" r:id="rId5" xr:uid="{5154C42F-7B7D-2849-B828-DF8BACE0B64D}"/>
-    <hyperlink ref="E10" r:id="rId6" xr:uid="{1A4292EE-D129-1D41-BE9E-1D35492C3E30}"/>
+    <hyperlink ref="E10" r:id="rId3" xr:uid="{F5E38187-B720-694E-8A41-E4D7CEA82071}"/>
+    <hyperlink ref="E9" r:id="rId4" xr:uid="{1A4292EE-D129-1D41-BE9E-1D35492C3E30}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{0F84FF7C-9D22-400A-9F0E-A9C8478304A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
     <tablePart r:id="rId7"/>
   </tableParts>
@@ -1589,7 +1622,7 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="15.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.5" style="11"/>
     <col min="2" max="2" width="13.6640625" style="11" customWidth="1"/>
@@ -1600,38 +1633,38 @@
     <col min="7" max="16384" width="15.5" style="11"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D3" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>62</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>72</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
@@ -1640,18 +1673,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C5" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>71</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>81</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
@@ -1660,18 +1693,18 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E6" s="3">
         <v>1</v>
@@ -1680,18 +1713,18 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -1700,18 +1733,18 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>70</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>80</v>
       </c>
       <c r="E8" s="3">
         <v>2</v>
@@ -1720,18 +1753,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
@@ -1740,18 +1773,18 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -1760,29 +1793,29 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="14">
+        <v>76</v>
+      </c>
+      <c r="E11" s="3">
         <v>1</v>
       </c>
       <c r="F11" s="7">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1809,7 +1842,7 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="20.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" style="1" customWidth="1"/>
@@ -1817,7 +1850,7 @@
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1837,18 +1870,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="93" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E5" s="7">
         <v>6.02</v>
@@ -1857,18 +1890,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="E6" s="7">
         <v>3.8</v>
@@ -1877,15 +1910,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="62" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2">
         <v>10022487</v>
@@ -1897,15 +1930,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="62" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D8" s="2">
         <v>10316140</v>
@@ -1917,18 +1950,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E9" s="10">
         <v>38.81</v>
@@ -1937,18 +1970,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="62" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E10" s="7">
         <v>86.4</v>
@@ -1957,9 +1990,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1970,7 +2003,7 @@
         <v>205.43</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1978,7 +2011,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1986,7 +2019,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1994,7 +2027,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2002,7 +2035,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2010,7 +2043,7 @@
       <c r="E16" s="7"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2018,7 +2051,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2026,7 +2059,7 @@
       <c r="E18" s="7"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2034,7 +2067,7 @@
       <c r="E19" s="7"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2042,7 +2075,7 @@
       <c r="E20" s="7"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2050,7 +2083,7 @@
       <c r="E21" s="7"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2058,7 +2091,7 @@
       <c r="E22" s="7"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>

</xml_diff>